<commit_message>
17,18: Add Sponsor Covenant & Sponsor Eligibility forms
</commit_message>
<xml_diff>
--- a/spec/fixtures/export_with_events/export_with_events.xlsx
+++ b/spec/fixtures/export_with_events/export_with_events.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -62,6 +62,12 @@
     <t>&lt;p&gt;&lt;em&gt;&lt;strong&gt;Confirmation Name&lt;/strong&gt;&lt;/em&gt;&lt;/p&gt;</t>
   </si>
   <si>
+    <t>Upload Sponsor Covenant</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;&lt;strong&gt;Upload Sponsor Covenant&lt;/strong&gt;&lt;/em&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>account_name</t>
   </si>
   <si>
@@ -135,6 +141,12 @@
   </si>
   <si>
     <t>candidate_events.5.verified</t>
+  </si>
+  <si>
+    <t>candidate_events.6.completed_date</t>
+  </si>
+  <si>
+    <t>candidate_events.6.verified</t>
   </si>
   <si>
     <t>vickikristoff</t>
@@ -1500,10 +1512,18 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>42674</v>
+      </c>
+      <c r="C8" s="4">
+        <v>42658</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>15</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
@@ -1542,7 +1562,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1573,120 +1593,128 @@
     <col min="23" max="23" width="18.6719" style="6" customWidth="1"/>
     <col min="24" max="24" width="18.6719" style="6" customWidth="1"/>
     <col min="25" max="25" width="18.6719" style="6" customWidth="1"/>
-    <col min="26" max="256" width="8.85156" style="6" customWidth="1"/>
+    <col min="26" max="26" width="18.6719" style="6" customWidth="1"/>
+    <col min="27" max="27" width="18.6719" style="6" customWidth="1"/>
+    <col min="28" max="256" width="8.85156" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K1" t="s" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L1" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M1" t="s" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O1" t="s" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P1" t="s" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Q1" t="s" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="R1" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="S1" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T1" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="U1" t="s" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V1" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="W1" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X1" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Y1" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="Z1" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA1" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="2" ht="14.6" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G2" s="3">
         <v>12</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s" s="2">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M2" s="3">
         <v>27502</v>
@@ -1717,41 +1745,45 @@
       <c r="Y2" t="b" s="7">
         <v>0</v>
       </c>
+      <c r="Z2" s="3"/>
+      <c r="AA2" t="b" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" ht="14.6" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G3" s="3">
         <v>9</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s" s="2">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M3" s="3">
         <v>27555</v>
@@ -1784,37 +1816,41 @@
       <c r="Y3" t="b" s="7">
         <v>0</v>
       </c>
+      <c r="Z3" s="4"/>
+      <c r="AA3" t="b" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" ht="14.6" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3">
         <v>10</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" t="s" s="2">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="M4" s="3">
         <v>47129</v>
@@ -1834,6 +1870,12 @@
       </c>
       <c r="Y4" t="b" s="7">
         <v>1</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>42736</v>
+      </c>
+      <c r="AA4" t="b" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="14.6" customHeight="1">
@@ -1862,6 +1904,8 @@
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
     </row>
     <row r="6" ht="14.6" customHeight="1">
       <c r="A6" s="3"/>
@@ -1889,6 +1933,8 @@
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
     </row>
     <row r="7" ht="14.6" customHeight="1">
       <c r="A7" s="3"/>
@@ -1916,6 +1962,8 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
       <c r="A8" s="3"/>
@@ -1943,6 +1991,8 @@
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
     </row>
     <row r="9" ht="14.6" customHeight="1">
       <c r="A9" s="3"/>
@@ -1970,6 +2020,8 @@
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
     </row>
     <row r="10" ht="14.6" customHeight="1">
       <c r="A10" s="3"/>
@@ -1997,6 +2049,8 @@
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
15, 16: removed old implementation of confirmation_name.
</commit_message>
<xml_diff>
--- a/spec/fixtures/export_with_events/export_with_events.xlsx
+++ b/spec/fixtures/export_with_events/export_with_events.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
   <si>
     <t>name</t>
   </si>
@@ -56,12 +56,6 @@
     <t>&lt;p&gt;&lt;em&gt;&lt;strong&gt;Upload certificate&lt;/strong&gt;&lt;/em&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>Confirmation Name</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;&lt;strong&gt;Confirmation Name&lt;/strong&gt;&lt;/em&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Upload Sponsor Covenant</t>
   </si>
   <si>
@@ -141,12 +135,6 @@
   </si>
   <si>
     <t>candidate_events.5.verified</t>
-  </si>
-  <si>
-    <t>candidate_events.6.completed_date</t>
-  </si>
-  <si>
-    <t>candidate_events.6.verified</t>
   </si>
   <si>
     <t>vickikristoff</t>
@@ -1384,7 +1372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1500,10 +1488,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="4">
-        <v>42643</v>
+        <v>42674</v>
       </c>
       <c r="C7" s="4">
-        <v>42625</v>
+        <v>42658</v>
       </c>
       <c r="D7" t="s" s="2">
         <v>13</v>
@@ -1512,18 +1500,10 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
-      <c r="A8" t="s" s="2">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4">
-        <v>42674</v>
-      </c>
-      <c r="C8" s="4">
-        <v>42658</v>
-      </c>
-      <c r="D8" t="s" s="2">
-        <v>15</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
@@ -1543,14 +1523,6 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" ht="14.6" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -1562,7 +1534,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1593,128 +1565,120 @@
     <col min="23" max="23" width="18.6719" style="6" customWidth="1"/>
     <col min="24" max="24" width="18.6719" style="6" customWidth="1"/>
     <col min="25" max="25" width="18.6719" style="6" customWidth="1"/>
-    <col min="26" max="26" width="18.6719" style="6" customWidth="1"/>
-    <col min="27" max="27" width="18.6719" style="6" customWidth="1"/>
-    <col min="28" max="256" width="8.85156" style="6" customWidth="1"/>
+    <col min="26" max="256" width="8.85156" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s" s="2">
         <v>16</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="D1" t="s" s="2">
         <v>17</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="E1" t="s" s="2">
         <v>18</v>
       </c>
-      <c r="D1" t="s" s="2">
+      <c r="F1" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="G1" t="s" s="2">
         <v>20</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="H1" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="I1" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="J1" t="s" s="2">
         <v>23</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="K1" t="s" s="2">
         <v>24</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="L1" t="s" s="2">
         <v>25</v>
       </c>
-      <c r="K1" t="s" s="2">
+      <c r="M1" t="s" s="2">
         <v>26</v>
       </c>
-      <c r="L1" t="s" s="2">
+      <c r="N1" t="s" s="2">
         <v>27</v>
       </c>
-      <c r="M1" t="s" s="2">
+      <c r="O1" t="s" s="2">
         <v>28</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="P1" t="s" s="2">
         <v>29</v>
       </c>
-      <c r="O1" t="s" s="2">
+      <c r="Q1" t="s" s="2">
         <v>30</v>
       </c>
-      <c r="P1" t="s" s="2">
+      <c r="R1" t="s" s="2">
         <v>31</v>
       </c>
-      <c r="Q1" t="s" s="2">
+      <c r="S1" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="R1" t="s" s="2">
+      <c r="T1" t="s" s="2">
         <v>33</v>
       </c>
-      <c r="S1" t="s" s="2">
+      <c r="U1" t="s" s="2">
         <v>34</v>
       </c>
-      <c r="T1" t="s" s="2">
+      <c r="V1" t="s" s="2">
         <v>35</v>
       </c>
-      <c r="U1" t="s" s="2">
+      <c r="W1" t="s" s="2">
         <v>36</v>
       </c>
-      <c r="V1" t="s" s="2">
+      <c r="X1" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="W1" t="s" s="2">
+      <c r="Y1" t="s" s="2">
         <v>38</v>
-      </c>
-      <c r="X1" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="Y1" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="Z1" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA1" t="s" s="2">
-        <v>42</v>
       </c>
     </row>
     <row r="2" ht="14.6" customHeight="1">
       <c r="A2" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s" s="2">
         <v>43</v>
       </c>
-      <c r="B2" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="E2" t="s" s="2">
-        <v>47</v>
-      </c>
       <c r="F2" t="s" s="2">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="G2" s="3">
         <v>12</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s" s="2">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M2" s="3">
         <v>27502</v>
@@ -1745,45 +1709,41 @@
       <c r="Y2" t="b" s="7">
         <v>0</v>
       </c>
-      <c r="Z2" s="3"/>
-      <c r="AA2" t="b" s="7">
-        <v>0</v>
-      </c>
     </row>
     <row r="3" ht="14.6" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G3" s="3">
         <v>9</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s" s="2">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M3" s="3">
         <v>27555</v>
@@ -1816,41 +1776,37 @@
       <c r="Y3" t="b" s="7">
         <v>0</v>
       </c>
-      <c r="Z3" s="4"/>
-      <c r="AA3" t="b" s="7">
-        <v>0</v>
-      </c>
     </row>
     <row r="4" ht="14.6" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3">
         <v>10</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" t="s" s="2">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M4" s="3">
         <v>47129</v>
@@ -1866,15 +1822,9 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="4">
-        <v>42729</v>
+        <v>42736</v>
       </c>
       <c r="Y4" t="b" s="7">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="4">
-        <v>42736</v>
-      </c>
-      <c r="AA4" t="b" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1904,8 +1854,6 @@
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
     </row>
     <row r="6" ht="14.6" customHeight="1">
       <c r="A6" s="3"/>
@@ -1933,8 +1881,6 @@
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
     </row>
     <row r="7" ht="14.6" customHeight="1">
       <c r="A7" s="3"/>
@@ -1962,8 +1908,6 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
       <c r="A8" s="3"/>
@@ -1991,8 +1935,6 @@
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
     </row>
     <row r="9" ht="14.6" customHeight="1">
       <c r="A9" s="3"/>
@@ -2020,8 +1962,6 @@
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
     </row>
     <row r="10" ht="14.6" customHeight="1">
       <c r="A10" s="3"/>
@@ -2049,8 +1989,6 @@
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
15, 16: added pick confirmation name event
</commit_message>
<xml_diff>
--- a/spec/fixtures/export_with_events/export_with_events.xlsx
+++ b/spec/fixtures/export_with_events/export_with_events.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
   <si>
     <t>name</t>
   </si>
@@ -62,6 +62,12 @@
     <t>&lt;p&gt;&lt;em&gt;&lt;strong&gt;Upload Sponsor Covenant&lt;/strong&gt;&lt;/em&gt;&lt;/p&gt;</t>
   </si>
   <si>
+    <t>Pick Confirmation Name</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;&lt;strong&gt;Pick Confirmation Name&lt;/strong&gt;&lt;/em&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>account_name</t>
   </si>
   <si>
@@ -135,6 +141,12 @@
   </si>
   <si>
     <t>candidate_events.5.verified</t>
+  </si>
+  <si>
+    <t>candidate_events.6.completed_date</t>
+  </si>
+  <si>
+    <t>candidate_events.6.verified</t>
   </si>
   <si>
     <t>vickikristoff</t>
@@ -1500,10 +1512,18 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" t="s" s="2">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4">
+        <v>42704</v>
+      </c>
+      <c r="C8" s="4">
+        <v>42694</v>
+      </c>
+      <c r="D8" t="s" s="2">
+        <v>15</v>
+      </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
@@ -1534,7 +1554,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1565,120 +1585,128 @@
     <col min="23" max="23" width="18.6719" style="6" customWidth="1"/>
     <col min="24" max="24" width="18.6719" style="6" customWidth="1"/>
     <col min="25" max="25" width="18.6719" style="6" customWidth="1"/>
-    <col min="26" max="256" width="8.85156" style="6" customWidth="1"/>
+    <col min="26" max="26" width="18.6719" style="6" customWidth="1"/>
+    <col min="27" max="27" width="18.6719" style="6" customWidth="1"/>
+    <col min="28" max="256" width="8.85156" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K1" t="s" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L1" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="M1" t="s" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="O1" t="s" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P1" t="s" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="Q1" t="s" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="R1" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="S1" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="T1" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="U1" t="s" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="V1" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="W1" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="X1" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Y1" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="Z1" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA1" t="s" s="2">
+        <v>42</v>
       </c>
     </row>
     <row r="2" ht="14.6" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G2" s="3">
         <v>12</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s" s="2">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M2" s="3">
         <v>27502</v>
@@ -1709,41 +1737,45 @@
       <c r="Y2" t="b" s="7">
         <v>0</v>
       </c>
+      <c r="Z2" s="3"/>
+      <c r="AA2" t="b" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" ht="14.6" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G3" s="3">
         <v>9</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s" s="2">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="M3" s="3">
         <v>27555</v>
@@ -1776,37 +1808,41 @@
       <c r="Y3" t="b" s="7">
         <v>0</v>
       </c>
+      <c r="Z3" s="4"/>
+      <c r="AA3" t="b" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" ht="14.6" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3">
         <v>10</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" t="s" s="2">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="M4" s="3">
         <v>47129</v>
@@ -1826,6 +1862,12 @@
       </c>
       <c r="Y4" t="b" s="7">
         <v>0</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>42729</v>
+      </c>
+      <c r="AA4" t="b" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="14.6" customHeight="1">
@@ -1854,6 +1896,8 @@
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
     </row>
     <row r="6" ht="14.6" customHeight="1">
       <c r="A6" s="3"/>
@@ -1881,6 +1925,8 @@
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
     </row>
     <row r="7" ht="14.6" customHeight="1">
       <c r="A7" s="3"/>
@@ -1908,6 +1954,8 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
       <c r="A8" s="3"/>
@@ -1935,6 +1983,8 @@
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
       <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
     </row>
     <row r="9" ht="14.6" customHeight="1">
       <c r="A9" s="3"/>
@@ -1962,6 +2012,8 @@
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
       <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
     </row>
     <row r="10" ht="14.6" customHeight="1">
       <c r="A10" s="3"/>
@@ -1989,6 +2041,8 @@
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
       <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
19: Add Conversation between Confirmation Sponsor and Candidate
</commit_message>
<xml_diff>
--- a/spec/fixtures/export_with_events/export_with_events.xlsx
+++ b/spec/fixtures/export_with_events/export_with_events.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
   <si>
     <t>name</t>
   </si>
@@ -68,6 +68,12 @@
     <t>&lt;p&gt;&lt;em&gt;&lt;strong&gt;Pick Confirmation Name&lt;/strong&gt;&lt;/em&gt;&lt;/p&gt;</t>
   </si>
   <si>
+    <t>Sponsor and Candidate Conversation</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;&lt;strong&gt;Sponsor Agreement&lt;/strong&gt;&lt;/em&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>account_name</t>
   </si>
   <si>
@@ -147,6 +153,12 @@
   </si>
   <si>
     <t>candidate_events.6.verified</t>
+  </si>
+  <si>
+    <t>candidate_events.7.completed_date</t>
+  </si>
+  <si>
+    <t>candidate_events.7.verified</t>
   </si>
   <si>
     <t>vickikristoff</t>
@@ -1528,10 +1540,18 @@
       <c r="F8" s="3"/>
     </row>
     <row r="9" ht="14.6" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4">
+        <v>42735</v>
+      </c>
+      <c r="C9" s="4">
+        <v>42719</v>
+      </c>
+      <c r="D9" t="s" s="2">
+        <v>17</v>
+      </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
@@ -1554,7 +1574,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1587,126 +1607,134 @@
     <col min="25" max="25" width="18.6719" style="6" customWidth="1"/>
     <col min="26" max="26" width="18.6719" style="6" customWidth="1"/>
     <col min="27" max="27" width="18.6719" style="6" customWidth="1"/>
-    <col min="28" max="256" width="8.85156" style="6" customWidth="1"/>
+    <col min="28" max="28" width="18.6719" style="6" customWidth="1"/>
+    <col min="29" max="29" width="18.6719" style="6" customWidth="1"/>
+    <col min="30" max="256" width="8.85156" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K1" t="s" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="L1" t="s" s="2">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="M1" t="s" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="O1" t="s" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="P1" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="Q1" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="R1" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="S1" t="s" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="T1" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="U1" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="V1" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="W1" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="X1" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Y1" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="Z1" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AA1" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="AB1" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC1" t="s" s="2">
+        <v>46</v>
       </c>
     </row>
     <row r="2" ht="14.6" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="G2" s="3">
         <v>12</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s" s="2">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="M2" s="3">
         <v>27502</v>
@@ -1741,41 +1769,45 @@
       <c r="AA2" t="b" s="7">
         <v>0</v>
       </c>
+      <c r="AB2" s="3"/>
+      <c r="AC2" t="b" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" ht="14.6" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G3" s="3">
         <v>9</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s" s="2">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="M3" s="3">
         <v>27555</v>
@@ -1812,37 +1844,41 @@
       <c r="AA3" t="b" s="7">
         <v>0</v>
       </c>
+      <c r="AB3" s="4"/>
+      <c r="AC3" t="b" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" ht="14.6" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3">
         <v>10</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" t="s" s="2">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="M4" s="3">
         <v>47129</v>
@@ -1868,6 +1904,12 @@
       </c>
       <c r="AA4" t="b" s="7">
         <v>1</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>42760</v>
+      </c>
+      <c r="AC4" t="b" s="7">
+        <v>0</v>
       </c>
     </row>
     <row r="5" ht="14.6" customHeight="1">
@@ -1898,6 +1940,8 @@
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
     </row>
     <row r="6" ht="14.6" customHeight="1">
       <c r="A6" s="3"/>
@@ -1927,6 +1971,8 @@
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
     </row>
     <row r="7" ht="14.6" customHeight="1">
       <c r="A7" s="3"/>
@@ -1956,6 +2002,8 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
       <c r="A8" s="3"/>
@@ -1985,6 +2033,8 @@
       <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
     </row>
     <row r="9" ht="14.6" customHeight="1">
       <c r="A9" s="3"/>
@@ -2014,6 +2064,8 @@
       <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
       <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
     </row>
     <row r="10" ht="14.6" customHeight="1">
       <c r="A10" s="3"/>
@@ -2043,6 +2095,8 @@
       <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
20: Add Christian Ministry Awareness Work & Form
</commit_message>
<xml_diff>
--- a/spec/fixtures/export_with_events/export_with_events.xlsx
+++ b/spec/fixtures/export_with_events/export_with_events.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t>name</t>
   </si>
@@ -74,6 +74,12 @@
     <t>&lt;p&gt;&lt;em&gt;&lt;strong&gt;Sponsor Agreement&lt;/strong&gt;&lt;/em&gt;&lt;/p&gt;</t>
   </si>
   <si>
+    <t>Christian Ministry Awareness</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;&lt;strong&gt;Christian Ministry Awareness&lt;/strong&gt;&lt;/em&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>account_name</t>
   </si>
   <si>
@@ -159,6 +165,12 @@
   </si>
   <si>
     <t>candidate_events.7.verified</t>
+  </si>
+  <si>
+    <t>candidate_events.8.completed_date</t>
+  </si>
+  <si>
+    <t>candidate_events.8.verified</t>
   </si>
   <si>
     <t>vickikristoff</t>
@@ -1556,10 +1568,18 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" ht="14.6" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="A10" t="s" s="2">
+        <v>18</v>
+      </c>
+      <c r="B10" s="4">
+        <v>42766</v>
+      </c>
+      <c r="C10" s="4">
+        <v>42757</v>
+      </c>
+      <c r="D10" t="s" s="2">
+        <v>19</v>
+      </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
@@ -1574,7 +1594,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AC10"/>
+  <dimension ref="A1:AE10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1609,132 +1629,140 @@
     <col min="27" max="27" width="18.6719" style="6" customWidth="1"/>
     <col min="28" max="28" width="18.6719" style="6" customWidth="1"/>
     <col min="29" max="29" width="18.6719" style="6" customWidth="1"/>
-    <col min="30" max="256" width="8.85156" style="6" customWidth="1"/>
+    <col min="30" max="30" width="18.6719" style="6" customWidth="1"/>
+    <col min="31" max="31" width="18.6719" style="6" customWidth="1"/>
+    <col min="32" max="256" width="8.85156" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.6" customHeight="1">
       <c r="A1" t="s" s="2">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="K1" t="s" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L1" t="s" s="2">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M1" t="s" s="2">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="O1" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="P1" t="s" s="2">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="Q1" t="s" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="R1" t="s" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="S1" t="s" s="2">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="T1" t="s" s="2">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="U1" t="s" s="2">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="V1" t="s" s="2">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="W1" t="s" s="2">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="X1" t="s" s="2">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Y1" t="s" s="2">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Z1" t="s" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="AA1" t="s" s="2">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AB1" t="s" s="2">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AC1" t="s" s="2">
-        <v>46</v>
+        <v>48</v>
+      </c>
+      <c r="AD1" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AE1" t="s" s="2">
+        <v>50</v>
       </c>
     </row>
     <row r="2" ht="14.6" customHeight="1">
       <c r="A2" t="s" s="2">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G2" s="3">
         <v>12</v>
       </c>
       <c r="H2" t="s" s="2">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="I2" t="s" s="2">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" t="s" s="2">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="L2" t="s" s="2">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="M2" s="3">
         <v>27502</v>
@@ -1773,41 +1801,45 @@
       <c r="AC2" t="b" s="7">
         <v>0</v>
       </c>
+      <c r="AD2" s="3"/>
+      <c r="AE2" t="b" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" ht="14.6" customHeight="1">
       <c r="A3" t="s" s="2">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F3" t="s" s="2">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G3" s="3">
         <v>9</v>
       </c>
       <c r="H3" t="s" s="2">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I3" t="s" s="2">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" t="s" s="2">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="L3" t="s" s="2">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="M3" s="3">
         <v>27555</v>
@@ -1848,37 +1880,41 @@
       <c r="AC3" t="b" s="7">
         <v>0</v>
       </c>
+      <c r="AD3" s="4"/>
+      <c r="AE3" t="b" s="7">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" ht="14.6" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s" s="2">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="3">
         <v>10</v>
       </c>
       <c r="H4" t="s" s="2">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" t="s" s="2">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="K4" t="s" s="2">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="L4" t="s" s="2">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="M4" s="3">
         <v>47129</v>
@@ -1909,6 +1945,10 @@
         <v>42760</v>
       </c>
       <c r="AC4" t="b" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="4"/>
+      <c r="AE4" t="b" s="7">
         <v>0</v>
       </c>
     </row>
@@ -1942,6 +1982,8 @@
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
       <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
     </row>
     <row r="6" ht="14.6" customHeight="1">
       <c r="A6" s="3"/>
@@ -1973,6 +2015,8 @@
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
     </row>
     <row r="7" ht="14.6" customHeight="1">
       <c r="A7" s="3"/>
@@ -2004,6 +2048,8 @@
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
     </row>
     <row r="8" ht="14.6" customHeight="1">
       <c r="A8" s="3"/>
@@ -2035,6 +2081,8 @@
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
     </row>
     <row r="9" ht="14.6" customHeight="1">
       <c r="A9" s="3"/>
@@ -2066,6 +2114,8 @@
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
     </row>
     <row r="10" ht="14.6" customHeight="1">
       <c r="A10" s="3"/>
@@ -2097,6 +2147,8 @@
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Converted candidate_sheet to its own class
</commit_message>
<xml_diff>
--- a/spec/fixtures/export_with_events/export_with_events.xlsx
+++ b/spec/fixtures/export_with_events/export_with_events.xlsx
@@ -83,40 +83,40 @@
     <t>account_name</t>
   </si>
   <si>
-    <t>first_name</t>
-  </si>
-  <si>
-    <t>last_name</t>
-  </si>
-  <si>
-    <t>candidate_email</t>
-  </si>
-  <si>
-    <t>parent_email_1</t>
-  </si>
-  <si>
-    <t>parent_email_2</t>
-  </si>
-  <si>
-    <t>grade</t>
-  </si>
-  <si>
-    <t>attending</t>
-  </si>
-  <si>
-    <t>address.street_1</t>
-  </si>
-  <si>
-    <t>address.street_2</t>
-  </si>
-  <si>
-    <t>address.city</t>
-  </si>
-  <si>
-    <t>address.state</t>
-  </si>
-  <si>
-    <t>address.zip_code</t>
+    <t>candidate_sheet.first_name</t>
+  </si>
+  <si>
+    <t>candidate_sheet.last_name</t>
+  </si>
+  <si>
+    <t>candidate_sheet.candidate_email</t>
+  </si>
+  <si>
+    <t>candidate_sheet.parent_email_1</t>
+  </si>
+  <si>
+    <t>candidate_sheet.parent_email_2</t>
+  </si>
+  <si>
+    <t>candidate_sheet.grade</t>
+  </si>
+  <si>
+    <t>candidate_sheet.attending</t>
+  </si>
+  <si>
+    <t>candidate_sheet.address.street_1</t>
+  </si>
+  <si>
+    <t>candidate_sheet.address.street_2</t>
+  </si>
+  <si>
+    <t>candidate_sheet.address.city</t>
+  </si>
+  <si>
+    <t>candidate_sheet.address.state</t>
+  </si>
+  <si>
+    <t>candidate_sheet.address.zip_code</t>
   </si>
   <si>
     <t>candidate_events.0.completed_date</t>

</xml_diff>